<commit_message>
correction to architect and data to dataset
</commit_message>
<xml_diff>
--- a/code/resources/dataset.xlsx
+++ b/code/resources/dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre Sempere\Documents\OC_P6\code\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierr\Documents\GitHub\OC_P6\code\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FD61B09-AF91-4AF8-AF98-938B5E861840}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3D9980-6080-4B19-864A-D0502A3A0C48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2EE8FE3C-81ED-4FBD-A3E9-588DBD79A97F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EE8FE3C-81ED-4FBD-A3E9-588DBD79A97F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="164">
   <si>
     <t>ORDER</t>
   </si>
@@ -105,9 +104,6 @@
     <t>STAFF</t>
   </si>
   <si>
-    <t>workplace</t>
-  </si>
-  <si>
     <t>restaurant_address_id</t>
   </si>
   <si>
@@ -163,16 +159,390 @@
   </si>
   <si>
     <t>restaurant_id</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Cole</t>
+  </si>
+  <si>
+    <t>Cassandra</t>
+  </si>
+  <si>
+    <t>Railly</t>
+  </si>
+  <si>
+    <t>Katarina</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Ramse</t>
+  </si>
+  <si>
+    <t>Theodore</t>
+  </si>
+  <si>
+    <t>Deacon</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Goines</t>
+  </si>
+  <si>
+    <t>Leland</t>
+  </si>
+  <si>
+    <t>id PFK</t>
+  </si>
+  <si>
+    <t>Cx</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Royce</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Marker</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Kirschner</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>630-555-1087</t>
+  </si>
+  <si>
+    <t>630-555-1319</t>
+  </si>
+  <si>
+    <t>101-555-1399</t>
+  </si>
+  <si>
+    <t>630-555-1663</t>
+  </si>
+  <si>
+    <t>510-555-1951</t>
+  </si>
+  <si>
+    <t>101-555-1453</t>
+  </si>
+  <si>
+    <t>510-555-9109</t>
+  </si>
+  <si>
+    <t>101-555-1301</t>
+  </si>
+  <si>
+    <t>510-555-9973</t>
+  </si>
+  <si>
+    <t>630-555-1949</t>
+  </si>
+  <si>
+    <t>510-555-9059</t>
+  </si>
+  <si>
+    <t>510-555-2003</t>
+  </si>
+  <si>
+    <t>101-555-9511</t>
+  </si>
+  <si>
+    <t>101-555-9743</t>
+  </si>
+  <si>
+    <t>630-555-1811</t>
+  </si>
+  <si>
+    <t>630-555-9199</t>
+  </si>
+  <si>
+    <t>630-555-9391</t>
+  </si>
+  <si>
+    <t>101-555-1997</t>
+  </si>
+  <si>
+    <t>101-555-1787</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Cooks</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>Adler</t>
+  </si>
+  <si>
+    <t>Vivan</t>
+  </si>
+  <si>
+    <t>Rutledge</t>
+  </si>
+  <si>
+    <t>Cashier</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Gale</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Whitley</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Foster</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+  </si>
+  <si>
+    <t>Slade</t>
+  </si>
+  <si>
+    <t>Hannah</t>
+  </si>
+  <si>
+    <t>Henri</t>
+  </si>
+  <si>
+    <t>Toussaint</t>
+  </si>
+  <si>
+    <t>West-VII_OCP</t>
+  </si>
+  <si>
+    <t>Markridge-Group_Pizza</t>
+  </si>
+  <si>
+    <t>Titan_OCP</t>
+  </si>
+  <si>
+    <t>630-555-1511</t>
+  </si>
+  <si>
+    <t>101-555-1579</t>
+  </si>
+  <si>
+    <t>510-555-1709</t>
+  </si>
+  <si>
+    <t>New-York</t>
+  </si>
+  <si>
+    <t>Emerson Plaza</t>
+  </si>
+  <si>
+    <t>Emerson Hotel - Room 607</t>
+  </si>
+  <si>
+    <t>South 52nd Street</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>New Brunswick ave.</t>
+  </si>
+  <si>
+    <t>Milburn ave.</t>
+  </si>
+  <si>
+    <t>Capitol Driveway NW</t>
+  </si>
+  <si>
+    <t>Washington DC</t>
+  </si>
+  <si>
+    <t>Senator Royce's office</t>
+  </si>
+  <si>
+    <t>J.D. Peoples Mental Hospital</t>
+  </si>
+  <si>
+    <t>Raritan Research Laboratory</t>
+  </si>
+  <si>
+    <t>james.cole@somemail.com</t>
+  </si>
+  <si>
+    <t>kyle.slade@mental.com</t>
+  </si>
+  <si>
+    <t>jennifer.goines@primary.com</t>
+  </si>
+  <si>
+    <t>katarina.wagner@something.ger</t>
+  </si>
+  <si>
+    <t>olivia.kirschner@witness.com</t>
+  </si>
+  <si>
+    <t>leland.frost@markridge.gouv</t>
+  </si>
+  <si>
+    <t>mantis@fakemail.com</t>
+  </si>
+  <si>
+    <t>julian.adler@mit-edu.com</t>
+  </si>
+  <si>
+    <t>marker.aaron@fake-senate.gouv</t>
+  </si>
+  <si>
+    <t>robet_gale@fbi.gouv</t>
+  </si>
+  <si>
+    <t>sen.royce@senate.gouv</t>
+  </si>
+  <si>
+    <t>henri_toussaint@cdc.org</t>
+  </si>
+  <si>
+    <t>hannah_jones@zeit.ger</t>
+  </si>
+  <si>
+    <t>cassie@cdc.org</t>
+  </si>
+  <si>
+    <t>peters.o@markridge.gouv</t>
+  </si>
+  <si>
+    <t>deacon@west7.com</t>
+  </si>
+  <si>
+    <t>ssg.whitley@spearhead.org</t>
+  </si>
+  <si>
+    <t>col.jonathan_foster@spearhead.com</t>
+  </si>
+  <si>
+    <t>jose_ramse@bff.com</t>
+  </si>
+  <si>
+    <t>Frost</t>
+  </si>
+  <si>
+    <t>some_hash_software_created</t>
+  </si>
+  <si>
+    <t>5th Ave At 23rd St</t>
+  </si>
+  <si>
+    <t>West VII Pizza</t>
+  </si>
+  <si>
+    <t>Elfreths Aly</t>
+  </si>
+  <si>
+    <t>Jefferson Dr SW</t>
+  </si>
+  <si>
+    <t>Titan_Pizzeria</t>
+  </si>
+  <si>
+    <t>Margherita</t>
+  </si>
+  <si>
+    <t>4 seasons</t>
+  </si>
+  <si>
+    <t>Veggie</t>
+  </si>
+  <si>
+    <t>Reina</t>
+  </si>
+  <si>
+    <t>4 fromaggi</t>
+  </si>
+  <si>
+    <t>tomato_sauce</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>ham</t>
+  </si>
+  <si>
+    <t>ing1</t>
+  </si>
+  <si>
+    <t>ing2</t>
+  </si>
+  <si>
+    <t>ing3</t>
+  </si>
+  <si>
+    <t>ing4</t>
+  </si>
+  <si>
+    <t>²</t>
+  </si>
+  <si>
+    <t>https://www.seashepherd.fr/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,13 +565,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -514,34 +888,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4840243-11FF-468E-9CD3-7CA2C4051191}">
-  <dimension ref="A1:BE8"/>
+  <dimension ref="A1:BH24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AX15" sqref="AX15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" customWidth="1"/>
-    <col min="28" max="28" width="9.42578125" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" customWidth="1"/>
-    <col min="32" max="32" width="17.7109375" customWidth="1"/>
-    <col min="37" max="37" width="14.140625" customWidth="1"/>
-    <col min="41" max="41" width="13.42578125" customWidth="1"/>
-    <col min="55" max="55" width="20.42578125" customWidth="1"/>
-    <col min="56" max="56" width="16.140625" customWidth="1"/>
-    <col min="57" max="57" width="23.85546875" customWidth="1"/>
+    <col min="9" max="9" width="34" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" customWidth="1"/>
+    <col min="21" max="21" width="24" customWidth="1"/>
+    <col min="22" max="22" width="28.5703125" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" customWidth="1"/>
+    <col min="28" max="28" width="16" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" customWidth="1"/>
+    <col min="31" max="31" width="27.140625" customWidth="1"/>
+    <col min="33" max="33" width="17.7109375" customWidth="1"/>
+    <col min="38" max="38" width="14.140625" customWidth="1"/>
+    <col min="42" max="42" width="13.42578125" customWidth="1"/>
+    <col min="45" max="45" width="18.140625" customWidth="1"/>
+    <col min="46" max="46" width="15.7109375" customWidth="1"/>
+    <col min="49" max="49" width="18.7109375" customWidth="1"/>
+    <col min="50" max="50" width="28.5703125" customWidth="1"/>
+    <col min="53" max="53" width="13.42578125" customWidth="1"/>
+    <col min="56" max="56" width="20.42578125" customWidth="1"/>
+    <col min="57" max="57" width="16.140625" customWidth="1"/>
+    <col min="58" max="58" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -551,34 +938,34 @@
       <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
-        <v>27</v>
-      </c>
-      <c r="X1" t="s">
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" t="s">
         <v>12</v>
       </c>
-      <c r="AF1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>0</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU1" t="s">
+      <c r="AR1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV1" t="s">
         <v>7</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BD1" t="s">
         <v>40</v>
       </c>
-      <c r="BC1" t="s">
-        <v>41</v>
-      </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -589,6 +976,9 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
       <c r="G3" t="s">
         <v>9</v>
       </c>
@@ -602,221 +992,1251 @@
         <v>11</v>
       </c>
       <c r="L3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S3" t="s">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
+      <c r="T3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>41</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>37</v>
+      </c>
+      <c r="BF3" t="s">
         <v>23</v>
       </c>
-      <c r="N3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
+    </row>
+    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T3" t="s">
-        <v>28</v>
-      </c>
-      <c r="U3" t="s">
-        <v>29</v>
-      </c>
-      <c r="V3" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="B4">
         <v>1</v>
       </c>
-      <c r="Y3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>28</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>37</v>
-      </c>
-      <c r="BC3" t="s">
+      <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="BD3" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="R4">
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" t="s">
+        <v>144</v>
+      </c>
+      <c r="L4">
+        <f>F19</f>
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="X4">
+      <c r="P4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4">
         <v>1</v>
       </c>
-      <c r="AI4">
+      <c r="T4">
+        <f>Y5</f>
+        <v>2</v>
+      </c>
+      <c r="U4" t="s">
+        <v>106</v>
+      </c>
+      <c r="V4" t="s">
+        <v>109</v>
+      </c>
+      <c r="W4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y4">
         <v>1</v>
       </c>
-      <c r="AQ4">
+      <c r="Z4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA4">
+        <v>31</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC4">
+        <v>7630</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ4">
         <v>1</v>
       </c>
-      <c r="AY4">
+      <c r="AR4">
         <v>1</v>
       </c>
+      <c r="AS4" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT4">
+        <v>7</v>
+      </c>
+      <c r="AV4">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ4">
+        <v>1</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="R5">
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J5" t="s">
+        <v>144</v>
+      </c>
+      <c r="L5">
+        <f>F9</f>
+        <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" t="s">
+        <v>143</v>
+      </c>
+      <c r="O5">
         <v>2</v>
       </c>
-      <c r="X5">
+      <c r="P5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>62</v>
+      </c>
+      <c r="S5">
         <v>2</v>
       </c>
-      <c r="AI5">
+      <c r="T5">
+        <f>Y8</f>
+        <v>5</v>
+      </c>
+      <c r="U5" t="s">
+        <v>107</v>
+      </c>
+      <c r="V5" t="s">
+        <v>110</v>
+      </c>
+      <c r="W5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y5">
         <v>2</v>
       </c>
-      <c r="AQ5">
+      <c r="Z5" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA5">
+        <v>175</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC5">
+        <v>7630</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AJ5">
         <v>2</v>
       </c>
-      <c r="AY5">
+      <c r="AR5">
         <v>2</v>
       </c>
+      <c r="AS5" t="s">
+        <v>151</v>
+      </c>
+      <c r="AT5">
+        <v>11</v>
+      </c>
+      <c r="AV5">
+        <v>2</v>
+      </c>
+      <c r="AX5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ5">
+        <v>2</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB5">
+        <v>1.2</v>
+      </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="R6">
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" t="s">
+        <v>144</v>
+      </c>
+      <c r="L6">
+        <f>F8</f>
+        <v>5</v>
+      </c>
+      <c r="M6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6">
         <v>3</v>
       </c>
-      <c r="X6">
+      <c r="P6" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>65</v>
+      </c>
+      <c r="S6">
         <v>3</v>
       </c>
-      <c r="AI6">
+      <c r="T6">
+        <f>Y12</f>
+        <v>9</v>
+      </c>
+      <c r="U6" t="s">
+        <v>108</v>
+      </c>
+      <c r="V6" t="s">
+        <v>111</v>
+      </c>
+      <c r="W6" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y6">
         <v>3</v>
       </c>
-      <c r="AQ6">
+      <c r="Z6" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA6">
+        <v>39000</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC6">
+        <v>42101</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ6">
         <v>3</v>
       </c>
-      <c r="AY6">
+      <c r="AR6">
         <v>3</v>
       </c>
+      <c r="AS6" t="s">
+        <v>152</v>
+      </c>
+      <c r="AT6">
+        <v>13</v>
+      </c>
+      <c r="AV6">
+        <v>3</v>
+      </c>
+      <c r="AX6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ6">
+        <v>3</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>157</v>
+      </c>
+      <c r="BB6">
+        <v>1.6</v>
+      </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
       <c r="F7">
         <v>4</v>
       </c>
-      <c r="R7">
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" t="s">
+        <v>144</v>
+      </c>
+      <c r="L7">
+        <f>F18</f>
+        <v>15</v>
+      </c>
+      <c r="M7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y7">
         <v>4</v>
       </c>
-      <c r="X7">
+      <c r="Z7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA7">
+        <v>530</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC7">
+        <v>7630</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>123</v>
+      </c>
+      <c r="AJ7">
         <v>4</v>
       </c>
-      <c r="AI7">
+      <c r="AR7">
         <v>4</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT7">
+        <v>13</v>
+      </c>
+      <c r="AV7">
         <v>4</v>
       </c>
-      <c r="AY7">
+      <c r="AX7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ7">
         <v>4</v>
       </c>
+      <c r="BA7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BB7">
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
       <c r="F8">
         <v>5</v>
       </c>
-      <c r="R8">
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8">
+        <f>F11</f>
+        <v>8</v>
+      </c>
+      <c r="M8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y8">
         <v>5</v>
       </c>
-      <c r="X8">
+      <c r="Z8" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA8">
+        <v>126</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC8">
+        <v>42101</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ8">
         <v>5</v>
       </c>
-      <c r="AI8">
+      <c r="AR8">
         <v>5</v>
       </c>
-      <c r="AQ8">
+      <c r="AS8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AT8">
+        <v>11</v>
+      </c>
+      <c r="AV8">
         <v>5</v>
       </c>
-      <c r="AY8">
+      <c r="AX8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AZ8">
         <v>5</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>159</v>
+      </c>
+      <c r="BB8">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" t="s">
+        <v>144</v>
+      </c>
+      <c r="L9">
+        <f>F10</f>
+        <v>7</v>
+      </c>
+      <c r="M9" t="s">
+        <v>91</v>
+      </c>
+      <c r="N9" t="s">
+        <v>92</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y9">
+        <v>6</v>
+      </c>
+      <c r="AJ9">
+        <v>6</v>
+      </c>
+      <c r="AX9" s="2"/>
+      <c r="AZ9">
+        <v>6</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BB9">
+        <v>1.7</v>
+      </c>
+      <c r="BH9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" t="s">
+        <v>144</v>
+      </c>
+      <c r="L10">
+        <f>F12</f>
+        <v>9</v>
+      </c>
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y10">
+        <v>7</v>
+      </c>
+      <c r="AJ10">
+        <v>7</v>
+      </c>
+      <c r="AZ10">
+        <v>7</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>161</v>
+      </c>
+      <c r="BB10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J11" t="s">
+        <v>144</v>
+      </c>
+      <c r="L11">
+        <f>F13</f>
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" t="s">
+        <v>95</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y11">
+        <v>8</v>
+      </c>
+      <c r="AJ11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J12" t="s">
+        <v>144</v>
+      </c>
+      <c r="L12">
+        <f>F22</f>
+        <v>19</v>
+      </c>
+      <c r="M12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y12">
+        <v>9</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA12">
+        <v>1000</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC12">
+        <v>20510</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J13" t="s">
+        <v>144</v>
+      </c>
+      <c r="L13">
+        <f>F20</f>
+        <v>17</v>
+      </c>
+      <c r="M13" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" t="s">
+        <v>97</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y13">
+        <v>10</v>
+      </c>
+      <c r="AJ13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" t="s">
+        <v>144</v>
+      </c>
+      <c r="L14">
+        <f>F21</f>
+        <v>18</v>
+      </c>
+      <c r="M14" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" t="s">
+        <v>99</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y14">
+        <v>11</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC14">
+        <v>20510</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J15" t="s">
+        <v>144</v>
+      </c>
+      <c r="L15">
+        <f>F5</f>
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>101</v>
+      </c>
+      <c r="N15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y15">
+        <v>12</v>
+      </c>
+      <c r="AJ15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" t="s">
+        <v>144</v>
+      </c>
+      <c r="L16">
+        <f>F16</f>
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>103</v>
+      </c>
+      <c r="N16" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y16">
+        <v>13</v>
+      </c>
+      <c r="AJ16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J17" t="s">
+        <v>144</v>
+      </c>
+      <c r="L17">
+        <f>F15</f>
+        <v>12</v>
+      </c>
+      <c r="M17" t="s">
+        <v>104</v>
+      </c>
+      <c r="N17" t="s">
+        <v>105</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y17">
+        <v>14</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA17">
+        <v>113</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC17">
+        <v>42101</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>15</v>
+      </c>
+      <c r="G18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y18">
+        <v>15</v>
+      </c>
+      <c r="AJ18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J19" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y19">
+        <v>16</v>
+      </c>
+      <c r="AJ19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J20" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y20">
+        <v>17</v>
+      </c>
+      <c r="AJ20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J21" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y21">
+        <v>18</v>
+      </c>
+      <c r="AJ21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>19</v>
+      </c>
+      <c r="G22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J22" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y22">
+        <v>19</v>
+      </c>
+      <c r="AJ22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="Y23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="6:36" x14ac:dyDescent="0.25">
+      <c r="Y24">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{824872D7-AA3A-4AF7-ABB0-644DE16002E8}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{75C00E83-4AA4-4A64-B34A-08EDF40A3D7C}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{7F46CD19-48F4-4607-8FD4-A7514982BC4E}"/>
+    <hyperlink ref="I7" r:id="rId4" xr:uid="{88CD4D62-F428-40C0-BA14-11628AC69E41}"/>
+    <hyperlink ref="I8" r:id="rId5" xr:uid="{0AA950F2-74F8-4D74-A3B6-3210E7EBE854}"/>
+    <hyperlink ref="I9" r:id="rId6" xr:uid="{152E7215-B568-4A55-B773-6D5477820E33}"/>
+    <hyperlink ref="I10" r:id="rId7" xr:uid="{2633D984-2C07-4AC4-94B7-5A6FCA0BFC4C}"/>
+    <hyperlink ref="I11" r:id="rId8" xr:uid="{A4E35E6E-8E4A-4C89-B8AE-734CB7BB81B4}"/>
+    <hyperlink ref="I12" r:id="rId9" xr:uid="{3D0C2FF2-4874-4D23-AED8-6C0273D4B92A}"/>
+    <hyperlink ref="I13" r:id="rId10" xr:uid="{C80E54CC-07B0-47E5-ABE0-988E5561C861}"/>
+    <hyperlink ref="I14" r:id="rId11" xr:uid="{2854F938-85DD-4B5A-99E8-1D34B96A4669}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{F43ED71B-C55E-4F32-B990-0270BDF34598}"/>
+    <hyperlink ref="I16" r:id="rId13" xr:uid="{3AC0697E-740C-4383-BE87-D01D2CC87D7B}"/>
+    <hyperlink ref="I17" r:id="rId14" xr:uid="{AA9AA975-1B17-4579-9AAF-4B2072E84362}"/>
+    <hyperlink ref="I18" r:id="rId15" xr:uid="{6093A781-48C9-47F0-9462-EC2562C7D8BB}"/>
+    <hyperlink ref="I19" r:id="rId16" xr:uid="{896BE7E5-24C7-41B6-BA3B-3F46A26090EF}"/>
+    <hyperlink ref="I20" r:id="rId17" xr:uid="{303B9348-5F73-46D1-82C6-BD60CA30E73A}"/>
+    <hyperlink ref="I21" r:id="rId18" xr:uid="{7B688344-3964-40AE-8C70-30630C63CE9E}"/>
+    <hyperlink ref="I22" r:id="rId19" xr:uid="{BD5BF1F7-0132-4B56-9CF9-C8C5EE8DC9B0}"/>
+    <hyperlink ref="AX4" r:id="rId20" xr:uid="{F08000CF-1CF5-4341-8F08-ED9059A2DEB3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update sql, PMD and dataset
</commit_message>
<xml_diff>
--- a/code/resources/dataset.xlsx
+++ b/code/resources/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre Sempere\Documents\OC_P6\code\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BAB4EB-EE56-44CE-9331-E2940D2A3782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6181C7C7-8526-4AC5-B0D1-34F22FF4140E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2EE8FE3C-81ED-4FBD-A3E9-588DBD79A97F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="183">
   <si>
     <t>ORDER</t>
   </si>
@@ -570,6 +570,18 @@
   </si>
   <si>
     <t>cream</t>
+  </si>
+  <si>
+    <t>1;2</t>
+  </si>
+  <si>
+    <t>1;2;3;4</t>
+  </si>
+  <si>
+    <t>1;4</t>
+  </si>
+  <si>
+    <t>1;2;3</t>
   </si>
 </sst>
 </file>
@@ -717,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -753,6 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1068,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4840243-11FF-468E-9CD3-7CA2C4051191}">
-  <dimension ref="A1:BF22"/>
+  <dimension ref="A1:BE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="102" workbookViewId="0">
+      <selection activeCell="AX11" sqref="AX11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1122,7 @@
     <col min="58" max="58" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1144,10 +1157,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>55</v>
       </c>
@@ -1284,17 +1297,14 @@
       <c r="BB3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BD3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE3" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="BE3" t="s">
-        <v>37</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1415,7 +1425,9 @@
       <c r="AV4" s="4">
         <v>1</v>
       </c>
-      <c r="AW4" s="5"/>
+      <c r="AW4" s="5" t="s">
+        <v>179</v>
+      </c>
       <c r="AX4" s="19" t="s">
         <v>158</v>
       </c>
@@ -1428,8 +1440,14 @@
       <c r="BB4" s="6">
         <v>1</v>
       </c>
+      <c r="BD4" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE4" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>14</v>
       </c>
@@ -1552,7 +1570,9 @@
       <c r="AV5" s="4">
         <v>2</v>
       </c>
-      <c r="AW5" s="5"/>
+      <c r="AW5" s="5" t="s">
+        <v>180</v>
+      </c>
       <c r="AX5" s="19" t="s">
         <v>158</v>
       </c>
@@ -1565,8 +1585,14 @@
       <c r="BB5" s="6">
         <v>1.2</v>
       </c>
+      <c r="BD5" s="4">
+        <v>2</v>
+      </c>
+      <c r="BE5" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1689,7 +1715,9 @@
       <c r="AV6" s="4">
         <v>3</v>
       </c>
-      <c r="AW6" s="5"/>
+      <c r="AW6" s="27" t="s">
+        <v>181</v>
+      </c>
       <c r="AX6" s="19" t="s">
         <v>158</v>
       </c>
@@ -1702,8 +1730,14 @@
       <c r="BB6" s="6">
         <v>1.6</v>
       </c>
+      <c r="BD6" s="4">
+        <v>3</v>
+      </c>
+      <c r="BE6" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
@@ -1810,7 +1844,9 @@
       <c r="AV7" s="4">
         <v>4</v>
       </c>
-      <c r="AW7" s="5"/>
+      <c r="AW7" s="27" t="s">
+        <v>182</v>
+      </c>
       <c r="AX7" s="19" t="s">
         <v>158</v>
       </c>
@@ -1823,8 +1859,14 @@
       <c r="BB7" s="6">
         <v>1.5</v>
       </c>
+      <c r="BD7" s="4">
+        <v>4</v>
+      </c>
+      <c r="BE7" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>11</v>
       </c>
@@ -1931,7 +1973,9 @@
       <c r="AV8" s="8">
         <v>5</v>
       </c>
-      <c r="AW8" s="9"/>
+      <c r="AW8" s="9" t="s">
+        <v>179</v>
+      </c>
       <c r="AX8" s="20" t="s">
         <v>158</v>
       </c>
@@ -1944,8 +1988,14 @@
       <c r="BB8" s="11">
         <v>1.9</v>
       </c>
+      <c r="BD8" s="4">
+        <v>5</v>
+      </c>
+      <c r="BE8" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F9" s="4">
         <v>6</v>
       </c>
@@ -2027,8 +2077,14 @@
       </c>
       <c r="AP9" s="6"/>
       <c r="AX9" s="1"/>
+      <c r="BD9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE9" s="6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F10" s="4">
         <v>7</v>
       </c>
@@ -2111,8 +2167,14 @@
       <c r="AP10" s="6" t="s">
         <v>172</v>
       </c>
+      <c r="BD10" s="4">
+        <v>2</v>
+      </c>
+      <c r="BE10" s="6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F11" s="4">
         <v>8</v>
       </c>
@@ -2191,8 +2253,14 @@
         <v>165</v>
       </c>
       <c r="AP11" s="6"/>
+      <c r="BD11" s="4">
+        <v>3</v>
+      </c>
+      <c r="BE11" s="6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F12" s="4">
         <v>9</v>
       </c>
@@ -2252,8 +2320,14 @@
         <v>165</v>
       </c>
       <c r="AP12" s="6"/>
+      <c r="BD12" s="4">
+        <v>4</v>
+      </c>
+      <c r="BE12" s="6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F13" s="4">
         <v>10</v>
       </c>
@@ -2315,8 +2389,14 @@
       <c r="AP13" s="6" t="s">
         <v>173</v>
       </c>
+      <c r="BD13" s="4">
+        <v>5</v>
+      </c>
+      <c r="BE13" s="6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F14" s="4">
         <v>11</v>
       </c>
@@ -2378,8 +2458,14 @@
       <c r="AP14" s="11" t="s">
         <v>174</v>
       </c>
+      <c r="BD14" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE14" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F15" s="4">
         <v>12</v>
       </c>
@@ -2414,8 +2500,14 @@
       <c r="Q15" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="BD15" s="4">
+        <v>2</v>
+      </c>
+      <c r="BE15" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="F16" s="4">
         <v>13</v>
       </c>
@@ -2450,8 +2542,14 @@
       <c r="Q16" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="BD16" s="4">
+        <v>3</v>
+      </c>
+      <c r="BE16" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:57" x14ac:dyDescent="0.25">
       <c r="F17" s="4">
         <v>14</v>
       </c>
@@ -2486,8 +2584,14 @@
       <c r="Q17" s="11" t="s">
         <v>65</v>
       </c>
+      <c r="BD17" s="4">
+        <v>4</v>
+      </c>
+      <c r="BE17" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:57" x14ac:dyDescent="0.25">
       <c r="F18" s="4">
         <v>15</v>
       </c>
@@ -2503,8 +2607,14 @@
       <c r="J18" s="6" t="s">
         <v>144</v>
       </c>
+      <c r="BD18" s="8">
+        <v>5</v>
+      </c>
+      <c r="BE18" s="11">
+        <v>3</v>
+      </c>
     </row>
-    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:57" x14ac:dyDescent="0.25">
       <c r="F19" s="4">
         <v>16</v>
       </c>
@@ -2521,7 +2631,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:57" x14ac:dyDescent="0.25">
       <c r="F20" s="4">
         <v>17</v>
       </c>
@@ -2538,7 +2648,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:57" x14ac:dyDescent="0.25">
       <c r="F21" s="4">
         <v>18</v>
       </c>
@@ -2555,7 +2665,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:57" x14ac:dyDescent="0.25">
       <c r="F22" s="8">
         <v>19</v>
       </c>

</xml_diff>